<commit_message>
Clean version 25/07 17h12
</commit_message>
<xml_diff>
--- a/Results_ALL.xlsx
+++ b/Results_ALL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0EE144DC-B3AB-4A50-82EE-0E7BF247A667}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E3CB0CA1-6766-4F7A-ADAB-5518AE94AE1E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CART_star,k=1" sheetId="4" r:id="rId1"/>
@@ -4449,7 +4449,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4563,7 +4563,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -20879,15 +20879,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
+      <xdr:colOff>300036</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>139387</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>426036</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>134625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25796,7 +25796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9CC4ED-481A-4276-B92E-DE7D3E54B79A}">
   <dimension ref="C3:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
@@ -26210,7 +26210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8638A96A-4360-4AFB-81B9-1DE0788597E7}">
   <dimension ref="B3:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>

</xml_diff>